<commit_message>
More firms. Small updates in other parts of the code. Added a DEFAULT VALUE to the SCOUT function
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/Sheet.xlsx
+++ b/src/main/resources/baseFiles/excel/Sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="93">
   <si>
     <t>Name</t>
   </si>
@@ -291,6 +291,21 @@
   </si>
   <si>
     <t>Horten</t>
+  </si>
+  <si>
+    <t>Dong Wu</t>
+  </si>
+  <si>
+    <t>wudong@huiyelaw.com</t>
+  </si>
+  <si>
+    <t>862152370950</t>
+  </si>
+  <si>
+    <t>https://www.huiyelaw.com/zyry-1.html</t>
+  </si>
+  <si>
+    <t>Huiye Law</t>
   </si>
 </sst>
 </file>
@@ -1397,7 +1412,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:J3"/>
@@ -1449,38 +1464,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="1">
-        <v>81</v>
-      </c>
-      <c r="B2" t="s" s="1">
-        <v>82</v>
-      </c>
-      <c r="C2" t="s" s="1">
-        <v>83</v>
-      </c>
-      <c r="D2" t="s" s="1">
-        <v>84</v>
-      </c>
-      <c r="E2" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="F2" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="G2" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s" s="3">
-        <v>26</v>
-      </c>
-      <c r="J2" t="s" s="2">
-        <v>87</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="+32 2 551 15 72" tooltip="https://liedekerke.com/en/lawyers/tel:+3225511572"/>

</xml_diff>

<commit_message>
Switching to the new structure - modify all the New Page sites
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/Sheet.xlsx
+++ b/src/main/resources/baseFiles/excel/Sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5000" uniqueCount="2236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5010" uniqueCount="2241">
   <si>
     <t>Name</t>
   </si>
@@ -6735,6 +6735,21 @@
   </si>
   <si>
     <t>DIMAC</t>
+  </si>
+  <si>
+    <t>Abi Frederick</t>
+  </si>
+  <si>
+    <t>abi.frederick@lewissilkin.com</t>
+  </si>
+  <si>
+    <t>962854</t>
+  </si>
+  <si>
+    <t>https://www.lewissilkin.com/experts/abi-frederick</t>
+  </si>
+  <si>
+    <t>Lewiss Silkin</t>
   </si>
 </sst>
 </file>
@@ -7841,7 +7856,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:J3"/>
@@ -7893,6 +7908,38 @@
         <v>9</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="1">
+        <v>2236</v>
+      </c>
+      <c r="B2" t="s" s="1">
+        <v>2237</v>
+      </c>
+      <c r="C2" t="s" s="1">
+        <v>2238</v>
+      </c>
+      <c r="D2" t="s" s="1">
+        <v>113</v>
+      </c>
+      <c r="E2" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s" s="2">
+        <v>2239</v>
+      </c>
+      <c r="G2" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s" s="3">
+        <v>152</v>
+      </c>
+      <c r="J2" t="s" s="2">
+        <v>2240</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="+32 2 551 15 72" tooltip="https://liedekerke.com/en/lawyers/tel:+3225511572"/>

</xml_diff>

<commit_message>
Excluded all the collected lawyers in previous iteration and month.txt
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/Sheet.xlsx
+++ b/src/main/resources/baseFiles/excel/Sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5010" uniqueCount="2241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5030" uniqueCount="2251">
   <si>
     <t>Name</t>
   </si>
@@ -6750,6 +6750,36 @@
   </si>
   <si>
     <t>Lewiss Silkin</t>
+  </si>
+  <si>
+    <t>Dalia Abbate</t>
+  </si>
+  <si>
+    <t>dabbate@pglex.it</t>
+  </si>
+  <si>
+    <t>3920022030305</t>
+  </si>
+  <si>
+    <t>https://pglex.it/en/professionals/dalia-abbate/</t>
+  </si>
+  <si>
+    <t>Pedersoli</t>
+  </si>
+  <si>
+    <t>Anthony M C Alexander</t>
+  </si>
+  <si>
+    <t>aalexander@dwpv.com</t>
+  </si>
+  <si>
+    <t>4163676920</t>
+  </si>
+  <si>
+    <t>https://www.dwpv.com/our-people/anthony-alexander</t>
+  </si>
+  <si>
+    <t>Davies Ward Phillips And Vineberg</t>
   </si>
 </sst>
 </file>
@@ -7910,22 +7940,22 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="1">
-        <v>2236</v>
+        <v>2246</v>
       </c>
       <c r="B2" t="s" s="1">
-        <v>2237</v>
+        <v>2247</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>2238</v>
+        <v>2248</v>
       </c>
       <c r="D2" t="s" s="1">
-        <v>113</v>
+        <v>157</v>
       </c>
       <c r="E2" t="s" s="2">
         <v>38</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>2239</v>
+        <v>2249</v>
       </c>
       <c r="G2" t="s" s="2">
         <v>16</v>
@@ -7934,10 +7964,10 @@
         <v>17</v>
       </c>
       <c r="I2" t="s" s="3">
-        <v>152</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>2240</v>
+        <v>2250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More one time usigin it
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/Sheet.xlsx
+++ b/src/main/resources/baseFiles/excel/Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="13480"/>
+    <workbookView windowWidth="29100" windowHeight="14460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1211,8 +1211,8 @@
   <sheetPr/>
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A424" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>

</xml_diff>

<commit_message>
Implementation of a CENTRAL logic of enableling and disableling continents
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/Sheet.xlsx
+++ b/src/main/resources/baseFiles/excel/Sheet.xlsx
@@ -1219,7 +1219,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M100"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:J496"/>
@@ -1228,57 +1228,35 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>9</v>
-      </c>
-    </row>
-    <row r="99" spans="11:13">
-      <c r="K99" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L99" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M99" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="100" spans="11:13">
-      <c r="K100" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L100" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M100" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More firms and adjustments in the driver instatiation on classes
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/Sheet.xlsx
+++ b/src/main/resources/baseFiles/excel/Sheet.xlsx
@@ -1218,34 +1218,34 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>9</v>
       </c>
     </row>

</xml_diff>